<commit_message>
latest updates: corrected outcome functions (censoring and survival times)
</commit_message>
<xml_diff>
--- a/simulation_settings.xlsx
+++ b/simulation_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wavel\OneDrive - Yale University\Documents\RWorkspace\coursework\BIS537\BIS537-Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C102545-B787-44AF-889E-5711F08500D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B404BF0-370E-4408-97BB-A4FB2A44DA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13230" yWindow="0" windowWidth="13335" windowHeight="15585" xr2:uid="{E03621E3-0F47-448B-A2E8-8A20EA0EB937}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E03621E3-0F47-448B-A2E8-8A20EA0EB937}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>alpha_0</t>
   </si>
@@ -113,10 +113,10 @@
     <t>low: 0.25</t>
   </si>
   <si>
-    <t>high: 2.696</t>
-  </si>
-  <si>
-    <t>low: 0.239</t>
+    <t>low: 0.228</t>
+  </si>
+  <si>
+    <t>high: 2.69</t>
   </si>
 </sst>
 </file>
@@ -290,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,20 +312,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,47 +641,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CC098B-B040-4822-9046-9D13859ED954}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="5" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="13"/>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="11" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="13"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -723,14 +725,17 @@
       <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -771,16 +776,20 @@
         <v>3</v>
       </c>
       <c r="N3" s="2">
-        <v>-3.95</v>
-      </c>
-      <c r="O3" s="14">
-        <v>2</v>
-      </c>
-      <c r="P3" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="O3" s="16">
+        <v>2</v>
+      </c>
+      <c r="P3" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="3">
+        <f>L3</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -821,16 +830,20 @@
         <v>3</v>
       </c>
       <c r="N4" s="2">
-        <v>-3.97</v>
-      </c>
-      <c r="O4" s="14">
-        <v>2</v>
-      </c>
-      <c r="P4" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="O4" s="16">
+        <v>2</v>
+      </c>
+      <c r="P4" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="3">
+        <f t="shared" ref="Q4:Q14" si="0">L4</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -871,16 +884,20 @@
         <v>3</v>
       </c>
       <c r="N5" s="2">
-        <v>-3.97</v>
-      </c>
-      <c r="O5" s="14">
-        <v>2</v>
-      </c>
-      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="16">
+        <v>2</v>
+      </c>
+      <c r="P5" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -897,7 +914,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F6" s="2">
-        <f>F3</f>
+        <f t="shared" ref="F6:F14" si="1">F3</f>
         <v>-0.05</v>
       </c>
       <c r="G6">
@@ -922,16 +939,20 @@
         <v>3</v>
       </c>
       <c r="N6" s="2">
-        <v>-3.94</v>
-      </c>
-      <c r="O6" s="14">
-        <v>2</v>
-      </c>
-      <c r="P6" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="O6" s="16">
+        <v>2</v>
+      </c>
+      <c r="P6" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -948,7 +969,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F7" s="2">
-        <f>F4</f>
+        <f t="shared" si="1"/>
         <v>-0.47499999999999998</v>
       </c>
       <c r="G7">
@@ -973,16 +994,20 @@
         <v>3</v>
       </c>
       <c r="N7" s="2">
-        <v>-3.95</v>
-      </c>
-      <c r="O7" s="14">
-        <v>2</v>
-      </c>
-      <c r="P7" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="O7" s="16">
+        <v>2</v>
+      </c>
+      <c r="P7" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -999,7 +1024,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F8" s="2">
-        <f>F5</f>
+        <f t="shared" si="1"/>
         <v>-1.43</v>
       </c>
       <c r="G8">
@@ -1024,16 +1049,20 @@
         <v>3</v>
       </c>
       <c r="N8" s="2">
-        <v>-3.94</v>
-      </c>
-      <c r="O8" s="14">
-        <v>2</v>
-      </c>
-      <c r="P8" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="O8" s="16">
+        <v>2</v>
+      </c>
+      <c r="P8" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -1050,7 +1079,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F9" s="2">
-        <f>F6</f>
+        <f t="shared" si="1"/>
         <v>-0.05</v>
       </c>
       <c r="G9">
@@ -1075,16 +1104,20 @@
         <v>3</v>
       </c>
       <c r="N9" s="2">
-        <v>-1.22</v>
-      </c>
-      <c r="O9" s="14">
-        <v>2</v>
-      </c>
-      <c r="P9" s="3">
+        <v>3.57</v>
+      </c>
+      <c r="O9" s="16">
+        <v>2</v>
+      </c>
+      <c r="P9" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1101,7 +1134,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F10" s="2">
-        <f>F7</f>
+        <f t="shared" si="1"/>
         <v>-0.47499999999999998</v>
       </c>
       <c r="G10">
@@ -1126,16 +1159,20 @@
         <v>3</v>
       </c>
       <c r="N10" s="2">
-        <v>-1.21</v>
-      </c>
-      <c r="O10" s="14">
-        <v>2</v>
-      </c>
-      <c r="P10" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="O10" s="16">
+        <v>2</v>
+      </c>
+      <c r="P10" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q10" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -1152,7 +1189,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F11" s="2">
-        <f>F8</f>
+        <f t="shared" si="1"/>
         <v>-1.43</v>
       </c>
       <c r="G11">
@@ -1177,16 +1214,20 @@
         <v>3</v>
       </c>
       <c r="N11" s="2">
-        <v>-1.22</v>
-      </c>
-      <c r="O11" s="14">
-        <v>2</v>
-      </c>
-      <c r="P11" s="3">
+        <v>3.54</v>
+      </c>
+      <c r="O11" s="16">
+        <v>2</v>
+      </c>
+      <c r="P11" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q11" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -1203,7 +1244,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F12" s="2">
-        <f>F9</f>
+        <f t="shared" si="1"/>
         <v>-0.05</v>
       </c>
       <c r="G12">
@@ -1228,16 +1269,20 @@
         <v>3</v>
       </c>
       <c r="N12" s="2">
-        <v>-1.18</v>
-      </c>
-      <c r="O12" s="14">
-        <v>2</v>
-      </c>
-      <c r="P12" s="3">
+        <v>3.71</v>
+      </c>
+      <c r="O12" s="16">
+        <v>2</v>
+      </c>
+      <c r="P12" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -1254,7 +1299,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F13" s="2">
-        <f>F10</f>
+        <f t="shared" si="1"/>
         <v>-0.47499999999999998</v>
       </c>
       <c r="G13">
@@ -1279,16 +1324,20 @@
         <v>3</v>
       </c>
       <c r="N13" s="2">
-        <v>-1.19</v>
-      </c>
-      <c r="O13" s="14">
-        <v>2</v>
-      </c>
-      <c r="P13" s="3">
+        <v>3.72</v>
+      </c>
+      <c r="O13" s="16">
+        <v>2</v>
+      </c>
+      <c r="P13" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13" s="3">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -1305,7 +1354,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F14" s="4">
-        <f>F11</f>
+        <f t="shared" si="1"/>
         <v>-1.43</v>
       </c>
       <c r="G14" s="5">
@@ -1330,16 +1379,20 @@
         <v>3</v>
       </c>
       <c r="N14" s="4">
-        <v>-1.2</v>
+        <v>3.71</v>
       </c>
       <c r="O14" s="5">
         <v>2</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="Q14" s="6">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
         <v>15</v>
       </c>
@@ -1347,17 +1400,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1366,9 +1419,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="N1:P1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>